<commit_message>
Initial use of Excel data
</commit_message>
<xml_diff>
--- a/host_data.xlsx
+++ b/host_data.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,15 +20,165 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="53">
   <si>
     <t xml:space="preserve">hostname</t>
   </si>
   <si>
-    <t xml:space="preserve">port1_ip_address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">port1_mask</t>
+    <t xml:space="preserve">ansible_network_os</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortios_access_token</t>
+  </si>
+  <si>
+    <t xml:space="preserve">group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mgmt_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timezone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port2_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port2_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port3_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port3_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lan_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lan_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lan_vlanid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmz_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmz_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dmz_vlanid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wireless_guest_ip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wireless_guest_alias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wireless_guest_vlanid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortinet.fortios.fortios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xpNccbqz1p3htjNdwNgnwy5qcr4nqb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.99.0.123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.0.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ-INT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.17.0.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ-INT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.1.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ-LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.2.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HQ-DMZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.0.3.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUEST-VLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spoke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.99.0.124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.1.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke1-INT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.17.1.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke1-INT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.1.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke1-LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1.3.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.99.0.125</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.16.2.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke2-INT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.17.2.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke2-INT2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.1.1/24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spoke2-LAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.2.3.1/24</t>
   </si>
 </sst>
 </file>
@@ -43,6 +193,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,9 +253,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -124,15 +279,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L11" activeCellId="0" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="15.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="18.24"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -144,6 +304,207 @@
       </c>
       <c r="C1" s="0" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="0" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>64</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="0" t="n">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP - including default outbound firewall policy
</commit_message>
<xml_diff>
--- a/host_data.xlsx
+++ b/host_data.xlsx
@@ -8,8 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Global" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="FWPolicy" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
   <si>
     <t xml:space="preserve">hostname</t>
   </si>
@@ -83,6 +82,36 @@
     <t xml:space="preserve">wireless_guest_vlanid</t>
   </si>
   <si>
+    <t xml:space="preserve">policyid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dest_int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dest_add</t>
+  </si>
+  <si>
+    <t xml:space="preserve">service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">action</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">logtraffic</t>
+  </si>
+  <si>
     <t xml:space="preserve">HQ</t>
   </si>
   <si>
@@ -131,6 +160,27 @@
     <t xml:space="preserve">GUEST-VLAN</t>
   </si>
   <si>
+    <t xml:space="preserve">Default-Outbound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">accept</t>
+  </si>
+  <si>
+    <t xml:space="preserve">always</t>
+  </si>
+  <si>
     <t xml:space="preserve">Spoke1</t>
   </si>
   <si>
@@ -189,21 +239,6 @@
   </si>
   <si>
     <t xml:space="preserve">10.2.3.1/24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest_int</t>
-  </si>
-  <si>
-    <t xml:space="preserve">source_add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest_add</t>
-  </si>
-  <si>
-    <t xml:space="preserve">service</t>
   </si>
 </sst>
 </file>
@@ -218,6 +253,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -307,20 +343,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:AD4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AD3" activeCellId="0" sqref="AD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="18.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="14.72"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,117 +422,177 @@
       <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="U1" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="0" t="n">
         <v>20</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="T2" s="0" t="n">
         <v>30</v>
+      </c>
+      <c r="U2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="N3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="T3" s="0" t="n">
         <v>30</v>
@@ -502,49 +600,49 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="N4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="T4" s="0" t="n">
         <v>30</v>
@@ -559,63 +657,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;A</oddHeader>
-    <oddFooter>&amp;CPage &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with FortiGate base config and tidy up some scripts/files
</commit_message>
<xml_diff>
--- a/host_data.xlsx
+++ b/host_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
   <si>
     <t xml:space="preserve">hostname</t>
   </si>
@@ -124,7 +124,7 @@
     <t xml:space="preserve">fortinet.fortios.fortios</t>
   </si>
   <si>
-    <t xml:space="preserve">mh8f39wbQ89H8brgq3k1kg9th1xb3p</t>
+    <t xml:space="preserve">GN1cH1bmb4t6yGt3qb7fwmknmwmNff</t>
   </si>
   <si>
     <t xml:space="preserve">hq</t>
@@ -169,10 +169,10 @@
     <t xml:space="preserve">GUEST-VLAN</t>
   </si>
   <si>
-    <t xml:space="preserve">Mgmt-Outbound</t>
-  </si>
-  <si>
-    <t xml:space="preserve">port1</t>
+    <t xml:space="preserve">Default-Outbound</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAN</t>
   </si>
   <si>
     <t xml:space="preserve">port2</t>
@@ -194,9 +194,6 @@
   </si>
   <si>
     <t xml:space="preserve">Spoke1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30zt4gdk7jf3k5NQmff06xhh4c9Qq4</t>
   </si>
   <si>
     <t xml:space="preserve">spoke</t>
@@ -357,14 +354,14 @@
   </sheetPr>
   <dimension ref="A1:AF4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O3" activeCellId="0" sqref="O3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.88"/>
@@ -478,7 +475,7 @@
       <c r="B2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>34</v>
       </c>
       <c r="D2" s="0" t="s">
@@ -576,14 +573,11 @@
       <c r="B3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>59</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>60</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>64</v>
@@ -595,28 +589,28 @@
         <v>38</v>
       </c>
       <c r="I3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="K3" s="0" t="s">
+      <c r="L3" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="L3" s="0" t="s">
+      <c r="M3" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="M3" s="0" t="s">
+      <c r="N3" s="0" t="s">
         <v>65</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>66</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T3" s="0" t="s">
         <v>48</v>
@@ -627,16 +621,16 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>33</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>64</v>
@@ -648,28 +642,28 @@
         <v>38</v>
       </c>
       <c r="I4" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>71</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>74</v>
-      </c>
-      <c r="N4" s="0" t="s">
-        <v>75</v>
       </c>
       <c r="O4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T4" s="0" t="s">
         <v>48</v>

</xml_diff>

<commit_message>
Updated routes script to use variables instead of hard coded
</commit_message>
<xml_diff>
--- a/host_data.xlsx
+++ b/host_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="83">
   <si>
     <t xml:space="preserve">hostname</t>
   </si>
@@ -85,6 +85,18 @@
     <t xml:space="preserve">wireless_guest_vlanid</t>
   </si>
   <si>
+    <t xml:space="preserve">route_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route_device</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route_gateway</t>
+  </si>
+  <si>
+    <t xml:space="preserve">route_destination</t>
+  </si>
+  <si>
     <t xml:space="preserve">policyid</t>
   </si>
   <si>
@@ -124,7 +136,7 @@
     <t xml:space="preserve">fortinet.fortios.fortios</t>
   </si>
   <si>
-    <t xml:space="preserve">GN1cH1bmb4t6yGt3qb7fwmknmwmNff</t>
+    <t xml:space="preserve">qnf7rQ95zy9frjpwH0tfHh0f9jQfw1</t>
   </si>
   <si>
     <t xml:space="preserve">hq</t>
@@ -167,6 +179,15 @@
   </si>
   <si>
     <t xml:space="preserve">GUEST-VLAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">port1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.99.0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0.0.0/0</t>
   </si>
   <si>
     <t xml:space="preserve">Default-Outbound</t>
@@ -352,22 +373,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF4"/>
+  <dimension ref="A1:AJ4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,7 +472,7 @@
       <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="0" t="s">
@@ -461,73 +484,85 @@
       <c r="AD1" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="0" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AF1" s="0" t="s">
         <v>31</v>
+      </c>
+      <c r="AG1" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" s="0" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O2" s="0" t="n">
         <v>10</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="R2" s="0" t="n">
         <v>20</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="U2" s="0" t="n">
         <v>30</v>
@@ -535,85 +570,97 @@
       <c r="V2" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="W2" s="2" t="s">
-        <v>49</v>
+      <c r="W2" s="0" t="s">
+        <v>53</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z2" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="AA2" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
+      </c>
+      <c r="Z2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AC2" s="0" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AD2" s="0" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AE2" s="0" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="AF2" s="0" t="s">
-        <v>56</v>
+        <v>60</v>
+      </c>
+      <c r="AG2" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="AH2" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI2" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ2" s="0" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="O3" s="0" t="n">
         <v>10</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="U3" s="0" t="n">
         <v>30</v>
@@ -621,52 +668,52 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>67</v>
+        <v>74</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>64</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="O4" s="0" t="n">
         <v>10</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>30</v>

</xml_diff>

<commit_message>
Updated menu with prompt for host to configure. Updated README
</commit_message>
<xml_diff>
--- a/host_data.xlsx
+++ b/host_data.xlsx
@@ -136,7 +136,7 @@
     <t xml:space="preserve">fortinet.fortios.fortios</t>
   </si>
   <si>
-    <t xml:space="preserve">qnf7rQ95zy9frjpwH0tfHh0f9jQfw1</t>
+    <t xml:space="preserve">j6wx0yh89kt7fkQ8qhmcnNshmQrzwp</t>
   </si>
   <si>
     <t xml:space="preserve">hq</t>
@@ -379,17 +379,17 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="21.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="18.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="18.61"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="13.24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="15.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="20.7"/>
   </cols>
   <sheetData>

</xml_diff>